<commit_message>
refactoring and fix error
</commit_message>
<xml_diff>
--- a/RaspisanieNew2/SozdanieRaspisaniya/bin/Debug/Расписание0.xlsx
+++ b/RaspisanieNew2/SozdanieRaspisaniya/bin/Debug/Расписание0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <x:si>
     <x:t>пр1</x:t>
   </x:si>
@@ -25,19 +25,16 @@
     <x:t>I 8:30 - 10:05</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">   группа2</x:t>
+    <x:t>предмет1   группа2</x:t>
   </x:si>
   <x:si>
     <x:t>II 10:20 - 11:55</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">   группа10</x:t>
+    <x:t xml:space="preserve">   </x:t>
   </x:si>
   <x:si>
     <x:t>III 12:10 - 13:45</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">   </x:t>
   </x:si>
   <x:si>
     <x:t>IV 14:15 - 15:50</x:t>
@@ -528,7 +525,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
@@ -537,10 +534,10 @@
     </x:row>
     <x:row r="8" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B8" s="2" t="s">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
@@ -549,10 +546,10 @@
     </x:row>
     <x:row r="10" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B10" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C10" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
@@ -561,10 +558,10 @@
     </x:row>
     <x:row r="12" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B12" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C12" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
@@ -573,13 +570,13 @@
     </x:row>
     <x:row r="14" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="A14" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B14" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C14" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
@@ -591,7 +588,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C16" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
@@ -603,7 +600,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C18" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
@@ -612,10 +609,10 @@
     </x:row>
     <x:row r="20" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B20" s="2" t="s">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C20" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
@@ -624,10 +621,10 @@
     </x:row>
     <x:row r="22" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B22" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C22" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
@@ -636,10 +633,10 @@
     </x:row>
     <x:row r="24" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B24" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C24" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
@@ -648,13 +645,13 @@
     </x:row>
     <x:row r="26" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="A26" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B26" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C26" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
@@ -666,7 +663,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C28" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
@@ -678,7 +675,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C30" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3">
@@ -687,10 +684,10 @@
     </x:row>
     <x:row r="32" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B32" s="2" t="s">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C32" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
@@ -699,10 +696,10 @@
     </x:row>
     <x:row r="34" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B34" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C34" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
@@ -710,10 +707,10 @@
     </x:row>
     <x:row r="36" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B36" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
@@ -721,13 +718,13 @@
     </x:row>
     <x:row r="38" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="A38" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B38" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:3">
@@ -738,7 +735,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3">
@@ -749,7 +746,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:3">
@@ -757,10 +754,10 @@
     </x:row>
     <x:row r="44" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B44" s="2" t="s">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:3">
@@ -768,10 +765,10 @@
     </x:row>
     <x:row r="46" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B46" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:3">
@@ -779,10 +776,10 @@
     </x:row>
     <x:row r="48" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B48" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:3">
@@ -790,13 +787,13 @@
     </x:row>
     <x:row r="50" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="A50" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B50" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:3">
@@ -807,7 +804,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:3">
@@ -818,7 +815,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:3">
@@ -826,10 +823,10 @@
     </x:row>
     <x:row r="56" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B56" s="2" t="s">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:3">
@@ -837,10 +834,10 @@
     </x:row>
     <x:row r="58" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B58" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:3">
@@ -848,10 +845,10 @@
     </x:row>
     <x:row r="60" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="B60" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:3">
@@ -859,13 +856,13 @@
     </x:row>
     <x:row r="62" spans="1:3" customFormat="1" ht="20" customHeight="1">
       <x:c r="A62" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B62" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:3">
@@ -876,7 +873,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:3">
@@ -887,7 +884,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:3">

</xml_diff>